<commit_message>
Updated genelists and genelist heatmap
</commit_message>
<xml_diff>
--- a/data/gene_lists/Gene lists Ribeiro et al 2025.xlsx
+++ b/data/gene_lists/Gene lists Ribeiro et al 2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ewallac2/Repos/cglab_rnaseq/data/gene_lists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A857D514-C8B0-2449-BA8E-8824A053FF00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688EE533-4279-064E-8152-215DA15A60E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" activeTab="1" xr2:uid="{45B065C0-E59E-4270-8E81-8C4DB542BCD8}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{45B065C0-E59E-4270-8E81-8C4DB542BCD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Delma_original" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="119">
   <si>
     <t>Azole/ergosterol specific</t>
   </si>
@@ -354,12 +354,75 @@
   <si>
     <t>Multi-drug transporter, aka CDR2</t>
   </si>
+  <si>
+    <t>ERG1</t>
+  </si>
+  <si>
+    <t>ERG2</t>
+  </si>
+  <si>
+    <t>ERG7</t>
+  </si>
+  <si>
+    <t>ERG24</t>
+  </si>
+  <si>
+    <t>ERG25</t>
+  </si>
+  <si>
+    <t>cell wall</t>
+  </si>
+  <si>
+    <t>stress response</t>
+  </si>
+  <si>
+    <t>SUN4</t>
+  </si>
+  <si>
+    <t>CAGL0F01463g</t>
+  </si>
+  <si>
+    <t>TIR1</t>
+  </si>
+  <si>
+    <t>Cell wall, mannoprotein</t>
+  </si>
+  <si>
+    <t>CAGL0C02211g</t>
+  </si>
+  <si>
+    <t>UTR2</t>
+  </si>
+  <si>
+    <t>Cell wall, transglycosidase, chitin incorporation</t>
+  </si>
+  <si>
+    <t>Cell wall biogenesis</t>
+  </si>
+  <si>
+    <t>CAGL0L05434g</t>
+  </si>
+  <si>
+    <t>CAGL0D05940g</t>
+  </si>
+  <si>
+    <t>CAGL0L10714g</t>
+  </si>
+  <si>
+    <t>CAGL0J10824g</t>
+  </si>
+  <si>
+    <t>CAGL0I02970g</t>
+  </si>
+  <si>
+    <t>CAGL0K04477g</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -391,6 +454,12 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -418,11 +487,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1101,10 +1171,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C15DAA-EC03-CD45-9DC2-57976A5432F0}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1186,22 +1256,22 @@
       <c r="A6" t="s">
         <v>64</v>
       </c>
-      <c r="B6" t="s">
-        <v>73</v>
+      <c r="B6" s="4" t="s">
+        <v>114</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>64</v>
       </c>
-      <c r="B7" t="s">
-        <v>84</v>
+      <c r="B7" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1209,10 +1279,10 @@
         <v>64</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1220,10 +1290,10 @@
         <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1231,80 +1301,65 @@
         <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" t="s">
-        <v>41</v>
+        <v>64</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s">
-        <v>55</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B14" t="s">
-        <v>71</v>
+        <v>64</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>117</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>55</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" t="s">
-        <v>76</v>
+        <v>64</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>118</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" t="s">
-        <v>55</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1312,10 +1367,10 @@
         <v>69</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D16" t="s">
         <v>55</v>
@@ -1326,13 +1381,13 @@
         <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>82</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1340,13 +1395,13 @@
         <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1354,13 +1409,13 @@
         <v>69</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1368,13 +1423,13 @@
         <v>69</v>
       </c>
       <c r="B20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1382,13 +1437,13 @@
         <v>69</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1396,13 +1451,13 @@
         <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C22" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D22" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1410,13 +1465,13 @@
         <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D23" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1424,13 +1479,13 @@
         <v>69</v>
       </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="C24" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1438,91 +1493,97 @@
         <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="B26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="D26" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28" t="s">
-        <v>12</v>
+        <v>103</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="C28" t="s">
-        <v>13</v>
+        <v>105</v>
       </c>
       <c r="D28" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>106</v>
+      </c>
+      <c r="C29" t="s">
+        <v>107</v>
       </c>
       <c r="D29" t="s">
-        <v>30</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>109</v>
+      </c>
+      <c r="C30" t="s">
+        <v>110</v>
       </c>
       <c r="D30" t="s">
-        <v>33</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="C31" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D31" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1530,13 +1591,10 @@
         <v>70</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D32" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1544,10 +1602,10 @@
         <v>70</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D33" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1555,13 +1613,13 @@
         <v>70</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C34" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D34" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1569,13 +1627,13 @@
         <v>70</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C35" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D35" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1583,7 +1641,7 @@
         <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D36" t="s">
         <v>30</v>
@@ -1594,10 +1652,13 @@
         <v>70</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="C37" t="s">
+        <v>46</v>
       </c>
       <c r="D37" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1605,10 +1666,13 @@
         <v>70</v>
       </c>
       <c r="B38" t="s">
-        <v>49</v>
+        <v>43</v>
+      </c>
+      <c r="C38" t="s">
+        <v>47</v>
       </c>
       <c r="D38" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1616,13 +1680,102 @@
         <v>70</v>
       </c>
       <c r="B39" t="s">
+        <v>44</v>
+      </c>
+      <c r="D39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>70</v>
+      </c>
+      <c r="B42" t="s">
         <v>50</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C42" t="s">
         <v>51</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D42" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>104</v>
+      </c>
+      <c r="B43" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>104</v>
+      </c>
+      <c r="B44" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" t="s">
+        <v>57</v>
+      </c>
+      <c r="D44" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>104</v>
+      </c>
+      <c r="B45" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>104</v>
+      </c>
+      <c r="B46" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" t="s">
+        <v>61</v>
+      </c>
+      <c r="D46" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>